<commit_message>
Implemented SEE - testing needed
</commit_message>
<xml_diff>
--- a/docs/LMR_Table.xlsx
+++ b/docs/LMR_Table.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_DEV\go\src\github.com\frankkopp\FrankyGo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_DEV\go\src\github.com\frankkopp\FrankyGo\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{899645EB-96AD-45B0-8AB8-2002190747A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F842B841-AA83-4690-8F3A-95D5CC1CB956}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11664" yWindow="249" windowWidth="28486" windowHeight="15617" xr2:uid="{AE6F5671-4308-494B-B7CB-D93DCDBACB2C}"/>
+    <workbookView xWindow="20605" yWindow="249" windowWidth="19545" windowHeight="15617" activeTab="1" xr2:uid="{AE6F5671-4308-494B-B7CB-D93DCDBACB2C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="LMR" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>Offset</t>
   </si>
@@ -42,6 +43,12 @@
   </si>
   <si>
     <t>Depth Factor</t>
+  </si>
+  <si>
+    <t>Pow</t>
+  </si>
+  <si>
+    <t>Base</t>
   </si>
 </sst>
 </file>
@@ -88,11 +95,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -409,8 +417,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD06691A-C22D-46B0-91A7-802D81CC893D}">
   <dimension ref="A1:BM30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -7774,4 +7782,328 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26D68186-A4B9-46FA-8E88-EBC64EFD32A9}">
+  <dimension ref="A1:E32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="11.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>4</v>
+      </c>
+      <c r="D1">
+        <v>1</v>
+      </c>
+      <c r="E1" s="4">
+        <f>$B$1+((D1+$B$2)^$B$3)</f>
+        <v>6.8284271247461898</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2" s="4">
+        <f t="shared" ref="E2:E32" si="0">$B$1+((D2+$B$2)^$B$3)</f>
+        <v>9.196152422706632</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>1.5</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3" s="4">
+        <f t="shared" si="0"/>
+        <v>11.999999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4" s="4">
+        <f t="shared" si="0"/>
+        <v>15.180339887498945</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5" s="4">
+        <f t="shared" si="0"/>
+        <v>18.696938456699073</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D6">
+        <v>6</v>
+      </c>
+      <c r="E6" s="4">
+        <f t="shared" si="0"/>
+        <v>22.520259177452129</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D7">
+        <v>7</v>
+      </c>
+      <c r="E7" s="4">
+        <f t="shared" si="0"/>
+        <v>26.627416997969508</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D8">
+        <v>8</v>
+      </c>
+      <c r="E8" s="4">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D9">
+        <v>9</v>
+      </c>
+      <c r="E9" s="4">
+        <f t="shared" si="0"/>
+        <v>35.622776601683803</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D10">
+        <v>10</v>
+      </c>
+      <c r="E10" s="4">
+        <f t="shared" si="0"/>
+        <v>40.482872693909407</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D11">
+        <v>11</v>
+      </c>
+      <c r="E11" s="4">
+        <f t="shared" si="0"/>
+        <v>45.56921938165307</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D12">
+        <v>12</v>
+      </c>
+      <c r="E12" s="4">
+        <f t="shared" si="0"/>
+        <v>50.87216658103187</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D13">
+        <v>13</v>
+      </c>
+      <c r="E13" s="4">
+        <f t="shared" si="0"/>
+        <v>56.383203414835151</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D14">
+        <v>14</v>
+      </c>
+      <c r="E14" s="4">
+        <f t="shared" si="0"/>
+        <v>62.094750193111238</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D15">
+        <v>15</v>
+      </c>
+      <c r="E15" s="4">
+        <f t="shared" si="0"/>
+        <v>67.999999999999972</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D16">
+        <v>16</v>
+      </c>
+      <c r="E16" s="4">
+        <f t="shared" si="0"/>
+        <v>74.092795635500266</v>
+      </c>
+    </row>
+    <row r="17" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D17">
+        <v>17</v>
+      </c>
+      <c r="E17" s="4">
+        <f t="shared" si="0"/>
+        <v>80.367532368147081</v>
+      </c>
+    </row>
+    <row r="18" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D18">
+        <v>18</v>
+      </c>
+      <c r="E18" s="4">
+        <f t="shared" si="0"/>
+        <v>86.819079927272767</v>
+      </c>
+    </row>
+    <row r="19" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D19">
+        <v>19</v>
+      </c>
+      <c r="E19" s="4">
+        <f t="shared" si="0"/>
+        <v>93.442719099991592</v>
+      </c>
+    </row>
+    <row r="20" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D20">
+        <v>20</v>
+      </c>
+      <c r="E20" s="4">
+        <f t="shared" si="0"/>
+        <v>100.23408959407267</v>
+      </c>
+    </row>
+    <row r="21" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D21">
+        <v>21</v>
+      </c>
+      <c r="E21" s="4">
+        <f t="shared" si="0"/>
+        <v>107.18914671611549</v>
+      </c>
+    </row>
+    <row r="22" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D22">
+        <v>22</v>
+      </c>
+      <c r="E22" s="4">
+        <f t="shared" si="0"/>
+        <v>114.30412503619254</v>
+      </c>
+    </row>
+    <row r="23" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D23">
+        <v>23</v>
+      </c>
+      <c r="E23" s="4">
+        <f t="shared" si="0"/>
+        <v>121.5755076535926</v>
+      </c>
+    </row>
+    <row r="24" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D24">
+        <v>24</v>
+      </c>
+      <c r="E24" s="4">
+        <f t="shared" si="0"/>
+        <v>128.99999999999994</v>
+      </c>
+    </row>
+    <row r="25" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D25">
+        <v>25</v>
+      </c>
+      <c r="E25" s="4">
+        <f t="shared" si="0"/>
+        <v>136.57450735341246</v>
+      </c>
+    </row>
+    <row r="26" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D26">
+        <v>26</v>
+      </c>
+      <c r="E26" s="4">
+        <f t="shared" si="0"/>
+        <v>144.29611541307906</v>
+      </c>
+    </row>
+    <row r="27" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D27">
+        <v>27</v>
+      </c>
+      <c r="E27" s="4">
+        <f t="shared" si="0"/>
+        <v>152.162073419617</v>
+      </c>
+    </row>
+    <row r="28" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D28">
+        <v>28</v>
+      </c>
+      <c r="E28" s="4">
+        <f t="shared" si="0"/>
+        <v>160.1697794069006</v>
+      </c>
+    </row>
+    <row r="29" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D29">
+        <v>29</v>
+      </c>
+      <c r="E29" s="4">
+        <f t="shared" si="0"/>
+        <v>168.31676725154981</v>
+      </c>
+    </row>
+    <row r="30" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D30">
+        <v>30</v>
+      </c>
+      <c r="E30" s="4">
+        <f t="shared" si="0"/>
+        <v>176.60069524773075</v>
+      </c>
+    </row>
+    <row r="31" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D31">
+        <v>31</v>
+      </c>
+      <c r="E31" s="4">
+        <f t="shared" si="0"/>
+        <v>185.01933598375612</v>
+      </c>
+    </row>
+    <row r="32" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D32">
+        <v>32</v>
+      </c>
+      <c r="E32" s="4">
+        <f t="shared" si="0"/>
+        <v>193.57056733575499</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>